<commit_message>
integration of codes and categories
</commit_message>
<xml_diff>
--- a/Rév8-codes.xlsx
+++ b/Rév8-codes.xlsx
@@ -193,10 +193,10 @@
     <t>Közös terek használata</t>
   </si>
   <si>
-    <t>Társadalmi sokszínűség (etnikai, osztálybeli, stb.)</t>
-  </si>
-  <si>
-    <t>Környezeti benyomások (zaj, szmog, stb)</t>
+    <t>Társadalmi sokszínűség (etnikai / osztálybeli / más)</t>
+  </si>
+  <si>
+    <t>Környezeti benyomások (zaj / szmog / más)</t>
   </si>
   <si>
     <t>Közterület használata</t>
@@ -208,7 +208,7 @@
     <t>Utca változásai</t>
   </si>
   <si>
-    <t>Lakossági összetétel, közösségek</t>
+    <t>Lakossági összetétel / közösségek</t>
   </si>
   <si>
     <t>Közbiztonság és közterületi viselkedés</t>

</xml_diff>